<commit_message>
My bot version 6.0 - added move ordering, increased search depth from 4 to 5, replaced evil bot with My bot version 6.0
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\Chess-Challange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58680729-F401-4901-87DE-96E4B6B47CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D5983-C5B6-4B2E-927D-B731040CC090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
   <si>
     <t>Random</t>
   </si>
@@ -411,9 +411,6 @@
     <t>1P Draw 2</t>
   </si>
   <si>
-    <t>Dynamic Depth</t>
-  </si>
-  <si>
     <t>r1bqkbnr/pp1ppppp/2n5/2p5/4P3/5N2/PPPP1PPP/RNBQKB1R w KQha - 0 1</t>
   </si>
   <si>
@@ -430,10 +427,6 @@
   </si>
   <si>
     <t>rnbqkbnr/pp1p1ppp/8/2p1p3/2P1P3/8/PP1P1PPP/RNBQKBNR w KQha - 0 1</t>
-  </si>
-  <si>
-    <t>Reduced brain
-rounded params to 5</t>
   </si>
   <si>
     <t>=-</t>
@@ -576,22 +569,42 @@
     <t>1058-904</t>
   </si>
   <si>
-    <t>sinus1</t>
-  </si>
-  <si>
-    <t>1055-1093</t>
-  </si>
-  <si>
-    <t>sinus1 v2</t>
-  </si>
-  <si>
-    <t>926-922</t>
-  </si>
-  <si>
-    <t>sinus1 v3</t>
-  </si>
-  <si>
-    <t>899-877</t>
+    <t>+- ?</t>
+  </si>
+  <si>
+    <t>for my own program - surrender button while testing -&gt; saves time</t>
+  </si>
+  <si>
+    <t>V5.5</t>
+  </si>
+  <si>
+    <t>1038-1060</t>
+  </si>
+  <si>
+    <t>668</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>math function for square array
+rescaled piece values</t>
+  </si>
+  <si>
+    <t>V6.0</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>move ordering
+depth 4-&gt;5</t>
+  </si>
+  <si>
+    <t>1246-1263</t>
   </si>
 </sst>
 </file>
@@ -640,7 +653,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,6 +687,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,9 +838,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -850,9 +866,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -904,6 +917,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1208,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,19 +1243,21 @@
     <col min="6" max="6" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.21875" style="7" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="7" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="9.21875" style="7" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="7"/>
+    <col min="19" max="19" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.21875" style="7" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1244,39 +1265,39 @@
         <v>1</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="J1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>124</v>
       </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1284,93 +1305,88 @@
         <v>2</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>136</v>
+      <c r="H2" s="31" t="s">
+        <v>134</v>
       </c>
       <c r="I2" s="11"/>
-      <c r="J2" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="18"/>
+      <c r="J2" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="6"/>
       <c r="N2" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="21">
-        <v>1</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="34">
+      <c r="L3" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="32">
         <v>1054</v>
       </c>
-      <c r="O3" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="P3" s="35">
-        <v>659</v>
-      </c>
-      <c r="Q3" s="35">
-        <v>661</v>
-      </c>
-      <c r="R3" s="35">
-        <v>668</v>
-      </c>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-    </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="O3" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
       <c r="B4" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1380,43 +1396,36 @@
       <c r="H4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="37"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="36">
+        <v>138</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="35">
         <v>1</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="37">
-        <v>0</v>
-      </c>
-      <c r="R4" s="37">
-        <v>3</v>
-      </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
       <c r="B5" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1424,34 +1433,33 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="37"/>
+      <c r="I5" s="35"/>
       <c r="J5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>153</v>
+        <v>139</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="N5" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q5" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="R5" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+        <v>168</v>
+      </c>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1467,45 +1475,38 @@
       <c r="H6" s="1">
         <v>18</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="35">
         <v>21</v>
       </c>
       <c r="J6" s="1">
         <v>20</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="35">
+        <v>15</v>
+      </c>
+      <c r="L6" s="35">
+        <v>28</v>
+      </c>
+      <c r="M6" s="1">
         <v>16</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="35">
         <v>20</v>
       </c>
-      <c r="M6" s="1">
-        <v>10</v>
-      </c>
-      <c r="N6" s="37">
-        <v>20</v>
-      </c>
       <c r="O6" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="P6" s="37">
-        <v>17</v>
-      </c>
-      <c r="Q6" s="37">
-        <v>16</v>
-      </c>
-      <c r="R6" s="37">
-        <v>13</v>
-      </c>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+        <v>166</v>
+      </c>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1521,45 +1522,38 @@
       <c r="H7" s="1">
         <v>7</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="35">
         <v>3</v>
       </c>
       <c r="J7" s="1">
         <v>4</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="35">
+        <v>9</v>
+      </c>
+      <c r="L7" s="35">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="L7" s="1">
-        <v>7</v>
-      </c>
-      <c r="M7" s="1">
-        <v>7</v>
-      </c>
-      <c r="N7" s="37">
+      <c r="N7" s="35">
         <v>1</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="37">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="37">
-        <v>9</v>
-      </c>
-      <c r="R7" s="37">
-        <v>7</v>
-      </c>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-      <c r="X7" s="37"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1577,197 +1571,181 @@
       <c r="H8" s="1">
         <v>13</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="35">
         <v>14</v>
       </c>
       <c r="J8" s="1">
         <v>14</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="35">
+        <v>14</v>
+      </c>
+      <c r="L8" s="35">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1">
         <v>16</v>
       </c>
-      <c r="L8" s="1">
-        <v>11</v>
-      </c>
-      <c r="M8" s="1">
-        <v>21</v>
-      </c>
-      <c r="N8" s="37">
+      <c r="N8" s="35">
         <v>17</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="P8" s="37">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="37">
-        <v>13</v>
-      </c>
-      <c r="R8" s="37">
-        <v>18</v>
-      </c>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+        <v>167</v>
+      </c>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="24">
-        <f t="shared" ref="E9:R9" si="0">SUM(E6:E8)</f>
+      <c r="E9" s="23">
+        <f t="shared" ref="E9:M9" si="0">SUM(E6:E8)</f>
         <v>38</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <f>SUM(H6:H8)</f>
         <v>38</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="36">
         <f>SUM(I6:I8)</f>
         <v>38</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="23">
         <f t="shared" ref="J9" si="1">SUM(J6:J8)</f>
         <v>38</v>
       </c>
-      <c r="K9" s="24">
-        <f t="shared" si="0"/>
+      <c r="K9" s="36">
+        <f t="shared" ref="K9:L9" si="2">SUM(K6:K8)</f>
         <v>38</v>
       </c>
-      <c r="L9" s="24">
-        <f t="shared" si="0"/>
+      <c r="L9" s="36">
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="M9" s="24">
-        <f>SUM(M6:M8)</f>
+      <c r="M9" s="23">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="23">
         <f>SUM(N6:N8)</f>
         <v>38</v>
       </c>
-      <c r="P9" s="38">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="Q9" s="38">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="R9" s="38">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-    </row>
-    <row r="10" spans="1:24" s="41" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40" t="s">
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+    </row>
+    <row r="10" spans="1:23" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="42">
-        <f t="shared" ref="E10:R10" si="2">(E6+E7/2)/E9</f>
+      <c r="E10" s="40">
+        <f t="shared" ref="E10:M10" si="3">(E6+E7/2)/E9</f>
         <v>1</v>
       </c>
-      <c r="F10" s="42">
-        <f t="shared" si="2"/>
+      <c r="F10" s="40">
+        <f t="shared" si="3"/>
         <v>0.86842105263157898</v>
       </c>
-      <c r="G10" s="42">
-        <f t="shared" si="2"/>
+      <c r="G10" s="40">
+        <f t="shared" si="3"/>
         <v>0.57894736842105265</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="40">
         <f>(H6+H7/2)/H9</f>
         <v>0.56578947368421051</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="40">
         <f>(I6+I7/2)/I9</f>
         <v>0.59210526315789469</v>
       </c>
-      <c r="J10" s="42">
-        <f t="shared" ref="J10" si="3">(J6+J7/2)/J9</f>
+      <c r="J10" s="40">
+        <f t="shared" ref="J10" si="4">(J6+J7/2)/J9</f>
         <v>0.57894736842105265</v>
       </c>
-      <c r="K10" s="42">
-        <f t="shared" si="2"/>
+      <c r="K10" s="40">
+        <f t="shared" ref="K10:L10" si="5">(K6+K7/2)/K9</f>
+        <v>0.51315789473684215</v>
+      </c>
+      <c r="L10" s="40">
+        <f t="shared" si="5"/>
+        <v>0.80263157894736847</v>
+      </c>
+      <c r="M10" s="40">
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L10" s="42">
-        <f t="shared" si="2"/>
-        <v>0.61842105263157898</v>
-      </c>
-      <c r="M10" s="42">
-        <f t="shared" si="2"/>
-        <v>0.35526315789473684</v>
-      </c>
-      <c r="N10" s="42">
-        <f t="shared" ref="N10" si="4">(N6+N7/2)/N9</f>
+      <c r="N10" s="40">
+        <f t="shared" ref="N10" si="6">(N6+N7/2)/N9</f>
         <v>0.53947368421052633</v>
       </c>
-      <c r="P10" s="42">
-        <f t="shared" si="2"/>
-        <v>0.52631578947368418</v>
-      </c>
-      <c r="Q10" s="42">
-        <f t="shared" si="2"/>
-        <v>0.53947368421052633</v>
-      </c>
-      <c r="R10" s="42">
-        <f t="shared" si="2"/>
-        <v>0.43421052631578949</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
+    </row>
+    <row r="11" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
+      <c r="N11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1794,12 +1772,15 @@
       <c r="K12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="M12" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
+      <c r="N12" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="21"/>
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1826,12 +1807,15 @@
       <c r="K13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="M13" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="N13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>111</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1860,12 +1844,15 @@
       <c r="K14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="M14" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="N14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1892,12 +1879,15 @@
       <c r="K15" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="M15" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="N15" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
@@ -1915,21 +1905,24 @@
         <v>16</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="M16" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="N16" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
@@ -1956,9 +1949,12 @@
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="M17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
@@ -1983,11 +1979,14 @@
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
       <c r="B19" s="6" t="s">
         <v>113</v>
       </c>
@@ -2003,12 +2002,12 @@
       <c r="J19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
+      <c r="K19" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
       <c r="B20" s="6" t="s">
         <v>114</v>
       </c>
@@ -2019,61 +2018,61 @@
       <c r="J20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="K20" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
       <c r="B21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="28" t="s">
-        <v>125</v>
+      <c r="H21" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="L21" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
+      <c r="J21" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
       <c r="B22" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="27" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="L22" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-    </row>
-    <row r="25" spans="1:12" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K22" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
+    </row>
+    <row r="25" spans="1:13" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>112</v>
       </c>
@@ -2094,10 +2093,17 @@
       <c r="H26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="6">
         <v>2</v>
@@ -2111,7 +2117,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="6" t="s">
         <v>22</v>
@@ -2127,7 +2133,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A11:XFD20">
+  <conditionalFormatting sqref="A11:S19 T11:XFD20 K11:L22 A20:R20 S20:S22">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>LEFT(A11,1)="-"</formula>
     </cfRule>
@@ -2148,7 +2154,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,7 +2253,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
@@ -2267,7 +2273,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -2287,7 +2293,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -2307,7 +2313,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
@@ -2321,7 +2327,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
@@ -2335,7 +2341,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -2460,7 +2466,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2486,7 +2492,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2494,7 +2500,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>60</v>
@@ -2510,50 +2516,53 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
-        <v>145</v>
+      <c r="A7" s="42" t="s">
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3566,53 +3575,53 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="43">
         <v>4</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="44">
         <v>3</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="44">
         <v>2</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="45">
         <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="41">
         <f>2*($F2)*(G$1)+ABS(G$7-$F8)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="41">
         <f t="shared" ref="H2:J2" si="0">2*($F2)*(H$1)+ABS(H$7-$F8)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="41">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="41">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="43">
+      <c r="L2" s="41">
         <f>ABS(B2-G2)</f>
         <v>4</v>
       </c>
-      <c r="M2" s="43">
+      <c r="M2" s="41">
         <f t="shared" ref="M2:O2" si="1">ABS(C2-H2)</f>
         <v>2</v>
       </c>
-      <c r="N2" s="43">
+      <c r="N2" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O2" s="43">
+      <c r="O2" s="41">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -3621,7 +3630,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="46">
         <v>3</v>
       </c>
       <c r="C3">
@@ -3630,48 +3639,48 @@
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="47">
         <v>5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="41">
         <f t="shared" ref="G3:J3" si="2">2*($F3)*(G$1)+ABS(G$7-$F9)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="41">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="41">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="41">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="41">
         <f t="shared" ref="L3:L5" si="3">ABS(B3-G3)</f>
         <v>2</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="41">
         <f t="shared" ref="M3:M5" si="4">ABS(C3-H3)</f>
         <v>5</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="41">
         <f t="shared" ref="N3:N5" si="5">ABS(D3-I3)</f>
         <v>1</v>
       </c>
-      <c r="O3" s="43">
+      <c r="O3" s="41">
         <f t="shared" ref="O3:O5" si="6">ABS(E3-J3)</f>
         <v>3</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="41">
         <f>SUM(L2:O5)</f>
         <v>44</v>
       </c>
@@ -3680,7 +3689,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="46">
         <v>2</v>
       </c>
       <c r="C4">
@@ -3689,44 +3698,44 @@
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="47">
         <v>8</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="41">
         <f t="shared" ref="G4:J4" si="7">2*($F4)*(G$1)+ABS(G$7-$F10)</f>
         <v>2</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="41">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="41">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="41">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="41">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="41">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="41">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="41">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -3735,53 +3744,53 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="48">
         <v>1</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="49">
         <v>5</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="49">
         <v>8</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="50">
         <v>10</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="41">
         <f t="shared" ref="G5:J5" si="8">2*($F5)*(G$1)+ABS(G$7-$F11)</f>
         <v>3</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="41">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="41">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="41">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="L5" s="43">
+      <c r="L5" s="41">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="41">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="41">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="O5" s="43">
+      <c r="O5" s="41">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
@@ -3828,53 +3837,53 @@
       <c r="A8">
         <v>0</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="43">
         <v>4</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="44">
         <v>3</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <v>2</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="45">
         <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="41">
         <f>4-ABS(G$7-$F8)+G$7*$F8</f>
         <v>4</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="41">
         <f t="shared" ref="H8:J11" si="9">4-ABS(H$7-$F8)+H$7*$F8</f>
         <v>3</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="41">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="41">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="41">
         <f>ABS(B8-G8)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="43">
+      <c r="M8" s="41">
         <f t="shared" ref="M8:M11" si="10">ABS(C8-H8)</f>
         <v>0</v>
       </c>
-      <c r="N8" s="43">
+      <c r="N8" s="41">
         <f t="shared" ref="N8:N11" si="11">ABS(D8-I8)</f>
         <v>0</v>
       </c>
-      <c r="O8" s="43">
+      <c r="O8" s="41">
         <f t="shared" ref="O8:O11" si="12">ABS(E8-J8)</f>
         <v>0</v>
       </c>
@@ -3883,7 +3892,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="46">
         <v>3</v>
       </c>
       <c r="C9">
@@ -3892,48 +3901,48 @@
       <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="47">
         <v>5</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="41">
         <f t="shared" ref="G9:G11" si="13">4-ABS(G$7-$F9)+G$7*$F9</f>
         <v>3</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="41">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="41">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="41">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="41">
         <f t="shared" ref="L9:L11" si="14">ABS(B9-G9)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="41">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="N9" s="43">
+      <c r="N9" s="41">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="41">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="Q9" s="41">
         <f>SUM(L8:O11)</f>
         <v>10</v>
       </c>
@@ -3942,7 +3951,7 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="46">
         <v>2</v>
       </c>
       <c r="C10">
@@ -3951,44 +3960,44 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="47">
         <v>8</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="41">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="41">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="41">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="41">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="41">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="41">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="41">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="41">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
@@ -3997,53 +4006,53 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="48">
         <v>1</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="49">
         <v>5</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="49">
         <v>8</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="50">
         <v>10</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="41">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="41">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="41">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="J11" s="43">
+      <c r="J11" s="41">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="41">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M11" s="43">
+      <c r="M11" s="41">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="41">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="41">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
@@ -4076,56 +4085,56 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" t="s">
         <v>158</v>
-      </c>
-      <c r="I15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K15" t="s">
-        <v>160</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="45">
+      <c r="N15" s="43">
         <v>1</v>
       </c>
-      <c r="O15" s="46">
+      <c r="O15" s="44">
         <v>2</v>
       </c>
-      <c r="P15" s="46">
+      <c r="P15" s="44">
         <v>3</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="45">
         <v>5</v>
       </c>
-      <c r="R15" s="45">
+      <c r="R15" s="43">
         <v>5</v>
       </c>
-      <c r="S15" s="46">
+      <c r="S15" s="44">
         <v>3</v>
       </c>
-      <c r="T15" s="46">
+      <c r="T15" s="44">
         <v>2</v>
       </c>
-      <c r="U15" s="47">
+      <c r="U15" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="46">
         <v>2</v>
       </c>
       <c r="O16">
@@ -4134,10 +4143,10 @@
       <c r="P16">
         <v>6</v>
       </c>
-      <c r="Q16" s="49">
+      <c r="Q16" s="47">
         <v>7</v>
       </c>
-      <c r="R16" s="48">
+      <c r="R16" s="46">
         <v>7</v>
       </c>
       <c r="S16">
@@ -4146,18 +4155,18 @@
       <c r="T16">
         <v>4</v>
       </c>
-      <c r="U16" s="49">
+      <c r="U16" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M17">
         <v>2</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="46">
         <v>3</v>
       </c>
       <c r="O17">
@@ -4166,10 +4175,10 @@
       <c r="P17">
         <v>8</v>
       </c>
-      <c r="Q17" s="49">
+      <c r="Q17" s="47">
         <v>9</v>
       </c>
-      <c r="R17" s="48">
+      <c r="R17" s="46">
         <v>9</v>
       </c>
       <c r="S17">
@@ -4178,71 +4187,71 @@
       <c r="T17">
         <v>6</v>
       </c>
-      <c r="U17" s="49">
+      <c r="U17" s="47">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="4:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M18">
         <v>3</v>
       </c>
-      <c r="N18" s="50">
+      <c r="N18" s="48">
         <v>5</v>
       </c>
-      <c r="O18" s="51">
+      <c r="O18" s="49">
         <v>7</v>
       </c>
-      <c r="P18" s="51">
+      <c r="P18" s="49">
         <v>9</v>
       </c>
-      <c r="Q18" s="52">
+      <c r="Q18" s="50">
         <v>10</v>
       </c>
-      <c r="R18" s="50">
+      <c r="R18" s="48">
         <v>10</v>
       </c>
-      <c r="S18" s="51">
+      <c r="S18" s="49">
         <v>9</v>
       </c>
-      <c r="T18" s="51">
+      <c r="T18" s="49">
         <v>7</v>
       </c>
-      <c r="U18" s="52">
+      <c r="U18" s="50">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M19">
         <v>4</v>
       </c>
-      <c r="N19" s="45">
+      <c r="N19" s="43">
         <v>5</v>
       </c>
-      <c r="O19" s="46">
+      <c r="O19" s="44">
         <v>7</v>
       </c>
-      <c r="P19" s="46">
+      <c r="P19" s="44">
         <v>9</v>
       </c>
-      <c r="Q19" s="47">
+      <c r="Q19" s="45">
         <v>10</v>
       </c>
-      <c r="R19" s="45">
+      <c r="R19" s="43">
         <v>10</v>
       </c>
-      <c r="S19" s="46">
+      <c r="S19" s="44">
         <v>9</v>
       </c>
-      <c r="T19" s="46">
+      <c r="T19" s="44">
         <v>7</v>
       </c>
-      <c r="U19" s="47">
+      <c r="U19" s="45">
         <v>5</v>
       </c>
     </row>
@@ -4250,7 +4259,7 @@
       <c r="M20">
         <v>5</v>
       </c>
-      <c r="N20" s="48">
+      <c r="N20" s="46">
         <v>3</v>
       </c>
       <c r="O20">
@@ -4259,10 +4268,10 @@
       <c r="P20">
         <v>8</v>
       </c>
-      <c r="Q20" s="49">
+      <c r="Q20" s="47">
         <v>9</v>
       </c>
-      <c r="R20" s="48">
+      <c r="R20" s="46">
         <v>9</v>
       </c>
       <c r="S20">
@@ -4271,7 +4280,7 @@
       <c r="T20">
         <v>6</v>
       </c>
-      <c r="U20" s="49">
+      <c r="U20" s="47">
         <v>3</v>
       </c>
     </row>
@@ -4279,7 +4288,7 @@
       <c r="M21">
         <v>6</v>
       </c>
-      <c r="N21" s="48">
+      <c r="N21" s="46">
         <v>2</v>
       </c>
       <c r="O21">
@@ -4288,10 +4297,10 @@
       <c r="P21">
         <v>6</v>
       </c>
-      <c r="Q21" s="49">
+      <c r="Q21" s="47">
         <v>7</v>
       </c>
-      <c r="R21" s="48">
+      <c r="R21" s="46">
         <v>7</v>
       </c>
       <c r="S21">
@@ -4300,7 +4309,7 @@
       <c r="T21">
         <v>4</v>
       </c>
-      <c r="U21" s="49">
+      <c r="U21" s="47">
         <v>2</v>
       </c>
     </row>
@@ -4308,28 +4317,28 @@
       <c r="M22">
         <v>7</v>
       </c>
-      <c r="N22" s="50">
+      <c r="N22" s="48">
         <v>1</v>
       </c>
-      <c r="O22" s="51">
+      <c r="O22" s="49">
         <v>2</v>
       </c>
-      <c r="P22" s="51">
+      <c r="P22" s="49">
         <v>3</v>
       </c>
-      <c r="Q22" s="52">
+      <c r="Q22" s="50">
         <v>5</v>
       </c>
-      <c r="R22" s="50">
+      <c r="R22" s="48">
         <v>5</v>
       </c>
-      <c r="S22" s="51">
+      <c r="S22" s="49">
         <v>3</v>
       </c>
-      <c r="T22" s="51">
+      <c r="T22" s="49">
         <v>2</v>
       </c>
-      <c r="U22" s="52">
+      <c r="U22" s="50">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reduced brain usage, excluded backward pawn evaluation
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\Chess-Challange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D5983-C5B6-4B2E-927D-B731040CC090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911FD6B0-62A5-4B90-A52F-33F5A9BC3DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="477" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparation" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="201">
   <si>
     <t>Random</t>
   </si>
@@ -560,12 +560,6 @@
     <t>1014</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>1058-904</t>
   </si>
   <si>
@@ -605,6 +599,72 @@
   </si>
   <si>
     <t>1246-1263</t>
+  </si>
+  <si>
+    <t>advanced pawn</t>
+  </si>
+  <si>
+    <t>255-249</t>
+  </si>
+  <si>
+    <t>no backwards</t>
+  </si>
+  <si>
+    <t>263-240</t>
+  </si>
+  <si>
+    <t>no isolated</t>
+  </si>
+  <si>
+    <t>no passed</t>
+  </si>
+  <si>
+    <t>no double</t>
+  </si>
+  <si>
+    <t>239-242</t>
+  </si>
+  <si>
+    <t>212-226</t>
+  </si>
+  <si>
+    <t>219-222</t>
+  </si>
+  <si>
+    <t>only backwards</t>
+  </si>
+  <si>
+    <t>only isolated</t>
+  </si>
+  <si>
+    <t>only passed</t>
+  </si>
+  <si>
+    <t>only double</t>
+  </si>
+  <si>
+    <t>239-227</t>
+  </si>
+  <si>
+    <t>220-255</t>
+  </si>
+  <si>
+    <t>977</t>
+  </si>
+  <si>
+    <t>243-265</t>
+  </si>
+  <si>
+    <t>213-222</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>1097</t>
+  </si>
+  <si>
+    <t>224-214</t>
   </si>
 </sst>
 </file>
@@ -791,7 +851,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -920,7 +980,22 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1227,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,26 +1313,34 @@
     <col min="1" max="1" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="27.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.21875" style="7" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="7" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.21875" style="7" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="7"/>
+    <col min="16" max="16" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.21875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.88671875" style="7"/>
+    <col min="27" max="27" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1283,10 +1366,10 @@
         <v>136</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>65</v>
@@ -1295,7 +1378,7 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:23" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>132</v>
       </c>
@@ -1318,23 +1401,55 @@
         <v>140</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L2" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
         <v>3</v>
@@ -1362,10 +1477,10 @@
         <v>137</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="32">
@@ -1374,16 +1489,38 @@
       <c r="O3" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-    </row>
-    <row r="4" spans="1:23" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="33">
+        <v>1097</v>
+      </c>
+      <c r="Q3" s="33">
+        <v>1088</v>
+      </c>
+      <c r="R3" s="33">
+        <v>1088</v>
+      </c>
+      <c r="S3" s="32">
+        <v>995</v>
+      </c>
+      <c r="T3" s="32">
+        <v>1088</v>
+      </c>
+      <c r="U3" s="32">
+        <v>977</v>
+      </c>
+      <c r="V3" s="32">
+        <v>977</v>
+      </c>
+      <c r="W3" s="32">
+        <v>1070</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
       <c r="B4" s="6" t="s">
         <v>125</v>
@@ -1401,10 +1538,10 @@
         <v>138</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="35">
@@ -1413,16 +1550,38 @@
       <c r="O4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="P4" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q4" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="S4" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="T4" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="U4" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="V4" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="W4" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="6" t="s">
         <v>126</v>
@@ -1438,170 +1597,258 @@
         <v>139</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N5" s="35" t="s">
         <v>151</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q5" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="U5" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="V5" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="W5" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="52">
         <v>38</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="52">
         <v>30</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="52">
         <v>17</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="52">
         <v>18</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="52">
         <v>21</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="52">
         <v>20</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="52">
         <v>15</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="52">
         <v>28</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="52">
         <v>16</v>
       </c>
-      <c r="N6" s="35">
+      <c r="N6" s="52">
         <v>20</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="2" t="s">
+      <c r="O6" s="52">
+        <v>16</v>
+      </c>
+      <c r="P6" s="52">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="52">
+        <v>18</v>
+      </c>
+      <c r="R6" s="52">
+        <v>15</v>
+      </c>
+      <c r="S6" s="52">
+        <v>16</v>
+      </c>
+      <c r="T6" s="52">
+        <v>14</v>
+      </c>
+      <c r="U6" s="52">
+        <v>13</v>
+      </c>
+      <c r="V6" s="52">
+        <v>19</v>
+      </c>
+      <c r="W6" s="52">
+        <v>21</v>
+      </c>
+      <c r="X6" s="52">
+        <v>15</v>
+      </c>
+      <c r="Z6" s="52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="52">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="52">
         <v>6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="52">
         <v>10</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="52">
         <v>7</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="52">
         <v>3</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="52">
         <v>4</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="52">
         <v>9</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="52">
         <v>5</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="52">
         <v>6</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="52">
         <v>1</v>
       </c>
-      <c r="O7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="O7" s="52">
+        <v>3</v>
+      </c>
+      <c r="P7" s="52">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="52">
+        <v>5</v>
+      </c>
+      <c r="R7" s="52">
+        <v>5</v>
+      </c>
+      <c r="S7" s="52">
+        <v>5</v>
+      </c>
+      <c r="T7" s="52">
+        <v>5</v>
+      </c>
+      <c r="U7" s="52">
+        <v>6</v>
+      </c>
+      <c r="V7" s="52">
+        <v>3</v>
+      </c>
+      <c r="W7" s="52">
+        <v>3</v>
+      </c>
+      <c r="X7" s="52">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="52">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="52">
         <v>2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="52">
         <v>11</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="52">
         <v>13</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="52">
         <v>14</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="52">
         <v>14</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="52">
         <v>14</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="52">
         <v>5</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="52">
         <v>16</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="52">
         <v>17</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O8" s="52">
+        <v>19</v>
+      </c>
+      <c r="P8" s="52">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="52">
+        <v>15</v>
+      </c>
+      <c r="R8" s="52">
+        <v>18</v>
+      </c>
+      <c r="S8" s="52">
+        <v>17</v>
+      </c>
+      <c r="T8" s="52">
+        <v>19</v>
+      </c>
+      <c r="U8" s="52">
+        <v>19</v>
+      </c>
+      <c r="V8" s="52">
+        <v>16</v>
+      </c>
+      <c r="W8" s="52">
+        <v>14</v>
+      </c>
+      <c r="X8" s="52">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="52">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -1646,30 +1893,74 @@
         <f>SUM(N6:N8)</f>
         <v>38</v>
       </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-    </row>
-    <row r="10" spans="1:23" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="23">
+        <f t="shared" ref="O9:P9" si="3">SUM(O6:O8)</f>
+        <v>38</v>
+      </c>
+      <c r="P9" s="23">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="Q9" s="23">
+        <f t="shared" ref="Q9" si="4">SUM(Q6:Q8)</f>
+        <v>38</v>
+      </c>
+      <c r="R9" s="23">
+        <f t="shared" ref="R9" si="5">SUM(R6:R8)</f>
+        <v>38</v>
+      </c>
+      <c r="S9" s="23">
+        <f t="shared" ref="S9" si="6">SUM(S6:S8)</f>
+        <v>38</v>
+      </c>
+      <c r="T9" s="23">
+        <f t="shared" ref="T9" si="7">SUM(T6:T8)</f>
+        <v>38</v>
+      </c>
+      <c r="U9" s="23">
+        <f t="shared" ref="U9" si="8">SUM(U6:U8)</f>
+        <v>38</v>
+      </c>
+      <c r="V9" s="23">
+        <f t="shared" ref="V9" si="9">SUM(V6:V8)</f>
+        <v>38</v>
+      </c>
+      <c r="W9" s="23">
+        <f t="shared" ref="W9" si="10">SUM(W6:W8)</f>
+        <v>38</v>
+      </c>
+      <c r="X9" s="23">
+        <f t="shared" ref="X9:Z9" si="11">SUM(X6:X8)</f>
+        <v>38</v>
+      </c>
+      <c r="Z9" s="23">
+        <f t="shared" si="11"/>
+        <v>38</v>
+      </c>
+      <c r="AA9" s="23">
+        <f t="shared" ref="AA9" si="12">SUM(AA6:AA8)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="23">
+        <f t="shared" ref="AB9" si="13">SUM(AB6:AB8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="37"/>
       <c r="B10" s="38" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="40">
-        <f t="shared" ref="E10:M10" si="3">(E6+E7/2)/E9</f>
+        <f t="shared" ref="E10:M10" si="14">(E6+E7/2)/E9</f>
         <v>1</v>
       </c>
       <c r="F10" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0.86842105263157898</v>
       </c>
       <c r="G10" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0.57894736842105265</v>
       </c>
       <c r="H10" s="40">
@@ -1681,31 +1972,79 @@
         <v>0.59210526315789469</v>
       </c>
       <c r="J10" s="40">
-        <f t="shared" ref="J10" si="4">(J6+J7/2)/J9</f>
+        <f t="shared" ref="J10" si="15">(J6+J7/2)/J9</f>
         <v>0.57894736842105265</v>
       </c>
       <c r="K10" s="40">
-        <f t="shared" ref="K10:L10" si="5">(K6+K7/2)/K9</f>
+        <f t="shared" ref="K10:L10" si="16">(K6+K7/2)/K9</f>
         <v>0.51315789473684215</v>
       </c>
       <c r="L10" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0.80263157894736847</v>
       </c>
       <c r="M10" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="N10" s="40">
-        <f t="shared" ref="N10" si="6">(N6+N7/2)/N9</f>
+        <f t="shared" ref="N10:P10" si="17">(N6+N7/2)/N9</f>
         <v>0.53947368421052633</v>
       </c>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-    </row>
-    <row r="11" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O10" s="40">
+        <f t="shared" si="17"/>
+        <v>0.46052631578947367</v>
+      </c>
+      <c r="P10" s="40">
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="40">
+        <f t="shared" ref="Q10:T10" si="18">(Q6+Q7/2)/Q9</f>
+        <v>0.53947368421052633</v>
+      </c>
+      <c r="R10" s="40">
+        <f t="shared" si="18"/>
+        <v>0.46052631578947367</v>
+      </c>
+      <c r="S10" s="40">
+        <f t="shared" si="18"/>
+        <v>0.48684210526315791</v>
+      </c>
+      <c r="T10" s="40">
+        <f t="shared" si="18"/>
+        <v>0.43421052631578949</v>
+      </c>
+      <c r="U10" s="40">
+        <f t="shared" ref="U10:X10" si="19">(U6+U7/2)/U9</f>
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="V10" s="40">
+        <f t="shared" si="19"/>
+        <v>0.53947368421052633</v>
+      </c>
+      <c r="W10" s="40">
+        <f t="shared" ref="W10:X10" si="20">(W6+W7/2)/W9</f>
+        <v>0.59210526315789469</v>
+      </c>
+      <c r="X10" s="40">
+        <f t="shared" si="20"/>
+        <v>0.43421052631578949</v>
+      </c>
+      <c r="Z10" s="40">
+        <f t="shared" ref="Z10:AB10" si="21">(Z6+Z7/2)/Z9</f>
+        <v>0.46052631578947367</v>
+      </c>
+      <c r="AA10" s="40" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB10" s="40" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
         <v>11</v>
@@ -1740,11 +2079,14 @@
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q11" s="53"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -1778,8 +2120,12 @@
       <c r="N12" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U12" s="27"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="53"/>
+      <c r="X12" s="27"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>
       <c r="B13" s="6" t="s">
         <v>13</v>
@@ -1814,7 +2160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>111</v>
       </c>
@@ -1851,7 +2197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -1886,7 +2232,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="6" t="s">
         <v>23</v>
@@ -1979,7 +2325,7 @@
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>18</v>
@@ -2035,7 +2381,7 @@
         <v>123</v>
       </c>
       <c r="K21" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2051,7 +2397,7 @@
         <v>17</v>
       </c>
       <c r="K22" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2547,7 +2893,7 @@
         <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
updateed stats excel file
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\Chess-Challange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911FD6B0-62A5-4B90-A52F-33F5A9BC3DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB427E6-4062-4483-99AB-B571935F38FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="477" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="202">
   <si>
     <t>Random</t>
   </si>
@@ -665,6 +665,10 @@
   </si>
   <si>
     <t>224-214</t>
+  </si>
+  <si>
+    <t>passed
+isolated</t>
   </si>
 </sst>
 </file>
@@ -713,7 +717,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +757,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,7 +867,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -997,6 +1013,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1304,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,9 +1402,16 @@
       <c r="M1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
@@ -1438,6 +1473,9 @@
       </c>
       <c r="X2" s="6" t="s">
         <v>192</v>
+      </c>
+      <c r="Y2" s="61" t="s">
+        <v>201</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>198</v>
@@ -1704,8 +1742,17 @@
       <c r="X6" s="52">
         <v>15</v>
       </c>
+      <c r="Y6" s="52">
+        <v>16</v>
+      </c>
       <c r="Z6" s="52">
         <v>16</v>
+      </c>
+      <c r="AA6" s="52">
+        <v>11</v>
+      </c>
+      <c r="AB6" s="52">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
@@ -1773,8 +1820,17 @@
       <c r="X7" s="52">
         <v>3</v>
       </c>
+      <c r="Y7" s="52">
+        <v>6</v>
+      </c>
       <c r="Z7" s="52">
         <v>3</v>
+      </c>
+      <c r="AA7" s="52">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="52">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
@@ -1844,8 +1900,17 @@
       <c r="X8" s="52">
         <v>20</v>
       </c>
+      <c r="Y8" s="52">
+        <v>16</v>
+      </c>
       <c r="Z8" s="52">
         <v>19</v>
+      </c>
+      <c r="AA8" s="52">
+        <v>24</v>
+      </c>
+      <c r="AB8" s="52">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
@@ -1933,17 +1998,21 @@
         <f t="shared" ref="X9:Z9" si="11">SUM(X6:X8)</f>
         <v>38</v>
       </c>
+      <c r="Y9" s="23">
+        <f t="shared" si="11"/>
+        <v>38</v>
+      </c>
       <c r="Z9" s="23">
         <f t="shared" si="11"/>
         <v>38</v>
       </c>
       <c r="AA9" s="23">
         <f t="shared" ref="AA9" si="12">SUM(AA6:AA8)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AB9" s="23">
         <f t="shared" ref="AB9" si="13">SUM(AB6:AB8)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2031,17 +2100,21 @@
         <f t="shared" si="20"/>
         <v>0.43421052631578949</v>
       </c>
+      <c r="Y10" s="40">
+        <f t="shared" ref="Y10" si="21">(Y6+Y7/2)/Y9</f>
+        <v>0.5</v>
+      </c>
       <c r="Z10" s="40">
-        <f t="shared" ref="Z10:AB10" si="21">(Z6+Z7/2)/Z9</f>
+        <f t="shared" ref="Z10:AB10" si="22">(Z6+Z7/2)/Z9</f>
         <v>0.46052631578947367</v>
       </c>
-      <c r="AA10" s="40" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB10" s="40" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
+      <c r="AA10" s="40">
+        <f t="shared" si="22"/>
+        <v>0.32894736842105265</v>
+      </c>
+      <c r="AB10" s="40">
+        <f t="shared" si="22"/>
+        <v>0.60526315789473684</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -2124,6 +2197,7 @@
       <c r="V12" s="53"/>
       <c r="W12" s="53"/>
       <c r="X12" s="27"/>
+      <c r="Y12" s="60"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>

</xml_diff>

<commit_message>
My bot version 7.0 - advanced pawn evaluation, minor tweaks, replaced evil bot with My bot version 7.0
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\Chess-Challange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB427E6-4062-4483-99AB-B571935F38FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9956F27B-A5D6-427A-A376-E63268252190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="477" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparation" sheetId="1" r:id="rId1"/>
     <sheet name="Testing" sheetId="2" r:id="rId2"/>
     <sheet name="Ideas" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Depth vs Breadth" sheetId="4" r:id="rId4"/>
+    <sheet name="Position array" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet2!$D$12:$D$13</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Position array'!$D$12:$D$13</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
@@ -34,7 +34,7 @@
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet2!$O$15</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Position array'!$O$15</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="201">
   <si>
     <t>Random</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>use time</t>
-  </si>
-  <si>
-    <t>pawn structure</t>
   </si>
   <si>
     <t>850/1024</t>
@@ -485,9 +482,6 @@
 results vs V4</t>
   </si>
   <si>
-    <t>transposition table - not recognize shortet mate</t>
-  </si>
-  <si>
     <t>castle points ?</t>
   </si>
   <si>
@@ -497,16 +491,10 @@
     <t>vary piece and positional value depending on endgame closeness</t>
   </si>
   <si>
-    <t>transposition check before or after mate ckeck?</t>
-  </si>
-  <si>
     <t>function intead of pos table ?</t>
   </si>
   <si>
     <t>king lee - maybe not needed</t>
-  </si>
-  <si>
-    <t>tuple instead of 3 arrays moves, value, depth</t>
   </si>
   <si>
     <t>TT</t>
@@ -658,9 +646,6 @@
     <t>213-222</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>1097</t>
   </si>
   <si>
@@ -669,6 +654,18 @@
   <si>
     <t>passed
 isolated</t>
+  </si>
+  <si>
+    <t>backward pawn evaluation</t>
+  </si>
+  <si>
+    <t>transposition table dictionary or array</t>
+  </si>
+  <si>
+    <t>all v2</t>
+  </si>
+  <si>
+    <t>V7.0</t>
   </si>
 </sst>
 </file>
@@ -867,7 +864,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -932,22 +929,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -996,28 +981,13 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1025,6 +995,15 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1330,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE23" sqref="AE22:AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,25 +1329,26 @@
     <col min="10" max="10" width="13.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="27.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.21875" style="7" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="7" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.21875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.88671875" style="7"/>
-    <col min="27" max="27" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="7" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" style="7" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" style="7" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="14.21875" style="7" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" style="7" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="11" style="7" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" style="7" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5546875" style="7" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" style="7" customWidth="1"/>
+    <col min="27" max="27" width="10.44140625" style="7" customWidth="1"/>
+    <col min="28" max="28" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1376,46 +1356,49 @@
         <v>1</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="Y1" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="6" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-    </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1423,68 +1406,68 @@
         <v>2</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>134</v>
+      <c r="H2" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="I2" s="11"/>
-      <c r="J2" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="31" t="s">
+      <c r="J2" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="M2" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="O2" s="6" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>181</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="T2" s="53" t="s">
+        <v>187</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="V2" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="W2" s="52" t="s">
+        <v>199</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="Y2" s="61" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>198</v>
+        <v>181</v>
+      </c>
+      <c r="Y2" s="27" t="s">
+        <v>177</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -1505,63 +1488,63 @@
         <v>32</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="33"/>
+        <v>126</v>
+      </c>
+      <c r="I3" s="29"/>
       <c r="J3" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K3" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="L3" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="32">
+      <c r="M3" s="29">
+        <v>1097</v>
+      </c>
+      <c r="N3" s="29">
+        <v>1088</v>
+      </c>
+      <c r="O3" s="29">
+        <v>1088</v>
+      </c>
+      <c r="P3" s="28">
+        <v>995</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>1088</v>
+      </c>
+      <c r="R3" s="28">
+        <v>977</v>
+      </c>
+      <c r="S3" s="28">
+        <v>977</v>
+      </c>
+      <c r="T3" s="28">
+        <v>1070</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="28">
         <v>1054</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="33">
-        <v>1097</v>
-      </c>
-      <c r="Q3" s="33">
-        <v>1088</v>
-      </c>
-      <c r="R3" s="33">
-        <v>1088</v>
-      </c>
-      <c r="S3" s="32">
-        <v>995</v>
-      </c>
-      <c r="T3" s="32">
-        <v>1088</v>
-      </c>
-      <c r="U3" s="32">
-        <v>977</v>
-      </c>
-      <c r="V3" s="32">
-        <v>977</v>
-      </c>
-      <c r="W3" s="32">
-        <v>1070</v>
-      </c>
-      <c r="X3" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>199</v>
+      <c r="AB3" s="19" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
       <c r="B4" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1571,58 +1554,58 @@
       <c r="H4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="L4" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="L4" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="35">
+      <c r="M4" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="P4" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="T4" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="31">
         <v>1</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="AB4" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="P4" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="R4" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="S4" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="T4" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="U4" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="V4" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="W4" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1630,287 +1613,287 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="35"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="K5" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="L5" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="N5" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="N5" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="P5" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q5" s="35" t="s">
+      <c r="O5" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="P5" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q5" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="R5" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="S5" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T5" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="U5" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="V5" s="35" t="s">
+      <c r="R5" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="S5" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="T5" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="W5" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z5" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="56" t="s">
+      <c r="U5" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA5" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="1">
         <v>38</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="1">
         <v>30</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="1">
         <v>17</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="1">
         <v>18</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="1">
         <v>21</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="1">
         <v>20</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="1">
         <v>15</v>
       </c>
-      <c r="L6" s="52">
+      <c r="L6" s="1">
         <v>28</v>
       </c>
-      <c r="M6" s="52">
+      <c r="M6" s="1">
         <v>16</v>
       </c>
-      <c r="N6" s="52">
+      <c r="N6" s="1">
+        <v>18</v>
+      </c>
+      <c r="O6" s="1">
+        <v>15</v>
+      </c>
+      <c r="P6" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>14</v>
+      </c>
+      <c r="R6" s="1">
+        <v>13</v>
+      </c>
+      <c r="S6" s="1">
+        <v>19</v>
+      </c>
+      <c r="T6" s="1">
+        <v>21</v>
+      </c>
+      <c r="U6" s="1">
+        <v>15</v>
+      </c>
+      <c r="V6" s="1">
+        <v>16</v>
+      </c>
+      <c r="W6" s="1">
+        <v>16</v>
+      </c>
+      <c r="X6" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="1">
         <v>20</v>
       </c>
-      <c r="O6" s="52">
+      <c r="Z6" s="1">
         <v>16</v>
       </c>
-      <c r="P6" s="52">
+      <c r="AA6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AB6" s="1">
         <v>16</v>
       </c>
-      <c r="Q6" s="52">
+    </row>
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1">
+        <v>6</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>5</v>
+      </c>
+      <c r="R7" s="1">
+        <v>6</v>
+      </c>
+      <c r="S7" s="1">
+        <v>3</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+      <c r="U7" s="1">
+        <v>3</v>
+      </c>
+      <c r="V7" s="1">
+        <v>6</v>
+      </c>
+      <c r="W7" s="1">
+        <v>3</v>
+      </c>
+      <c r="X7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1">
+        <v>14</v>
+      </c>
+      <c r="K8" s="1">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1">
+        <v>16</v>
+      </c>
+      <c r="N8" s="1">
+        <v>15</v>
+      </c>
+      <c r="O8" s="1">
         <v>18</v>
       </c>
-      <c r="R6" s="52">
-        <v>15</v>
-      </c>
-      <c r="S6" s="52">
+      <c r="P8" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>19</v>
+      </c>
+      <c r="R8" s="1">
+        <v>19</v>
+      </c>
+      <c r="S8" s="1">
         <v>16</v>
       </c>
-      <c r="T6" s="52">
+      <c r="T8" s="1">
         <v>14</v>
       </c>
-      <c r="U6" s="52">
-        <v>13</v>
-      </c>
-      <c r="V6" s="52">
+      <c r="U8" s="1">
+        <v>20</v>
+      </c>
+      <c r="V8" s="1">
+        <v>16</v>
+      </c>
+      <c r="W8" s="1">
         <v>19</v>
       </c>
-      <c r="W6" s="52">
-        <v>21</v>
-      </c>
-      <c r="X6" s="52">
-        <v>15</v>
-      </c>
-      <c r="Y6" s="52">
+      <c r="X8" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="1">
         <v>16</v>
       </c>
-      <c r="Z6" s="52">
-        <v>16</v>
-      </c>
-      <c r="AA6" s="52">
-        <v>11</v>
-      </c>
-      <c r="AB6" s="52">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="52">
-        <v>0</v>
-      </c>
-      <c r="F7" s="52">
-        <v>6</v>
-      </c>
-      <c r="G7" s="52">
-        <v>10</v>
-      </c>
-      <c r="H7" s="52">
-        <v>7</v>
-      </c>
-      <c r="I7" s="52">
-        <v>3</v>
-      </c>
-      <c r="J7" s="52">
-        <v>4</v>
-      </c>
-      <c r="K7" s="52">
-        <v>9</v>
-      </c>
-      <c r="L7" s="52">
-        <v>5</v>
-      </c>
-      <c r="M7" s="52">
-        <v>6</v>
-      </c>
-      <c r="N7" s="52">
-        <v>1</v>
-      </c>
-      <c r="O7" s="52">
-        <v>3</v>
-      </c>
-      <c r="P7" s="52">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="52">
-        <v>5</v>
-      </c>
-      <c r="R7" s="52">
-        <v>5</v>
-      </c>
-      <c r="S7" s="52">
-        <v>5</v>
-      </c>
-      <c r="T7" s="52">
-        <v>5</v>
-      </c>
-      <c r="U7" s="52">
-        <v>6</v>
-      </c>
-      <c r="V7" s="52">
-        <v>3</v>
-      </c>
-      <c r="W7" s="52">
-        <v>3</v>
-      </c>
-      <c r="X7" s="52">
-        <v>3</v>
-      </c>
-      <c r="Y7" s="52">
-        <v>6</v>
-      </c>
-      <c r="Z7" s="52">
-        <v>3</v>
-      </c>
-      <c r="AA7" s="52">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="52">
-        <v>0</v>
-      </c>
-      <c r="F8" s="52">
-        <v>2</v>
-      </c>
-      <c r="G8" s="52">
-        <v>11</v>
-      </c>
-      <c r="H8" s="52">
-        <v>13</v>
-      </c>
-      <c r="I8" s="52">
-        <v>14</v>
-      </c>
-      <c r="J8" s="52">
-        <v>14</v>
-      </c>
-      <c r="K8" s="52">
-        <v>14</v>
-      </c>
-      <c r="L8" s="52">
-        <v>5</v>
-      </c>
-      <c r="M8" s="52">
-        <v>16</v>
-      </c>
-      <c r="N8" s="52">
+      <c r="AA8" s="1">
         <v>17</v>
       </c>
-      <c r="O8" s="52">
+      <c r="AB8" s="1">
         <v>19</v>
-      </c>
-      <c r="P8" s="52">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="52">
-        <v>15</v>
-      </c>
-      <c r="R8" s="52">
-        <v>18</v>
-      </c>
-      <c r="S8" s="52">
-        <v>17</v>
-      </c>
-      <c r="T8" s="52">
-        <v>19</v>
-      </c>
-      <c r="U8" s="52">
-        <v>19</v>
-      </c>
-      <c r="V8" s="52">
-        <v>16</v>
-      </c>
-      <c r="W8" s="52">
-        <v>14</v>
-      </c>
-      <c r="X8" s="52">
-        <v>20</v>
-      </c>
-      <c r="Y8" s="52">
-        <v>16</v>
-      </c>
-      <c r="Z8" s="52">
-        <v>19</v>
-      </c>
-      <c r="AA8" s="52">
-        <v>24</v>
-      </c>
-      <c r="AB8" s="52">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
@@ -1919,7 +1902,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="23">
-        <f t="shared" ref="E9:M9" si="0">SUM(E6:E8)</f>
+        <f t="shared" ref="E9:G9" si="0">SUM(E6:E8)</f>
         <v>38</v>
       </c>
       <c r="F9" s="23">
@@ -1934,7 +1917,7 @@
         <f>SUM(H6:H8)</f>
         <v>38</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="32">
         <f>SUM(I6:I8)</f>
         <v>38</v>
       </c>
@@ -1942,179 +1925,179 @@
         <f t="shared" ref="J9" si="1">SUM(J6:J8)</f>
         <v>38</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="32">
         <f t="shared" ref="K9:L9" si="2">SUM(K6:K8)</f>
         <v>38</v>
       </c>
-      <c r="L9" s="36">
+      <c r="L9" s="32">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="M9" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M9" si="3">SUM(M6:M8)</f>
         <v>38</v>
       </c>
       <c r="N9" s="23">
-        <f>SUM(N6:N8)</f>
+        <f t="shared" ref="N9" si="4">SUM(N6:N8)</f>
         <v>38</v>
       </c>
       <c r="O9" s="23">
-        <f t="shared" ref="O9:P9" si="3">SUM(O6:O8)</f>
+        <f t="shared" ref="O9" si="5">SUM(O6:O8)</f>
         <v>38</v>
       </c>
       <c r="P9" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="P9" si="6">SUM(P6:P8)</f>
         <v>38</v>
       </c>
       <c r="Q9" s="23">
-        <f t="shared" ref="Q9" si="4">SUM(Q6:Q8)</f>
+        <f t="shared" ref="Q9" si="7">SUM(Q6:Q8)</f>
         <v>38</v>
       </c>
       <c r="R9" s="23">
-        <f t="shared" ref="R9" si="5">SUM(R6:R8)</f>
+        <f t="shared" ref="R9" si="8">SUM(R6:R8)</f>
         <v>38</v>
       </c>
       <c r="S9" s="23">
-        <f t="shared" ref="S9" si="6">SUM(S6:S8)</f>
+        <f t="shared" ref="S9" si="9">SUM(S6:S8)</f>
         <v>38</v>
       </c>
       <c r="T9" s="23">
-        <f t="shared" ref="T9" si="7">SUM(T6:T8)</f>
+        <f t="shared" ref="T9" si="10">SUM(T6:T8)</f>
         <v>38</v>
       </c>
       <c r="U9" s="23">
-        <f t="shared" ref="U9" si="8">SUM(U6:U8)</f>
+        <f t="shared" ref="U9:W9" si="11">SUM(U6:U8)</f>
         <v>38</v>
       </c>
       <c r="V9" s="23">
-        <f t="shared" ref="V9" si="9">SUM(V6:V8)</f>
-        <v>38</v>
-      </c>
-      <c r="W9" s="23">
-        <f t="shared" ref="W9" si="10">SUM(W6:W8)</f>
-        <v>38</v>
-      </c>
-      <c r="X9" s="23">
-        <f t="shared" ref="X9:Z9" si="11">SUM(X6:X8)</f>
-        <v>38</v>
-      </c>
-      <c r="Y9" s="23">
         <f t="shared" si="11"/>
         <v>38</v>
       </c>
-      <c r="Z9" s="23">
+      <c r="W9" s="23">
         <f t="shared" si="11"/>
         <v>38</v>
       </c>
+      <c r="X9" s="23">
+        <f t="shared" ref="X9" si="12">SUM(X6:X8)</f>
+        <v>38</v>
+      </c>
+      <c r="Y9" s="23">
+        <f t="shared" ref="Y9" si="13">SUM(Y6:Y8)</f>
+        <v>38</v>
+      </c>
+      <c r="Z9" s="23">
+        <f t="shared" ref="Z9:AB9" si="14">SUM(Z6:Z8)</f>
+        <v>38</v>
+      </c>
       <c r="AA9" s="23">
-        <f t="shared" ref="AA9" si="12">SUM(AA6:AA8)</f>
+        <f>SUM(AA6:AA8)</f>
         <v>38</v>
       </c>
       <c r="AB9" s="23">
-        <f t="shared" ref="AB9" si="13">SUM(AB6:AB8)</f>
+        <f t="shared" ref="AB9" si="15">SUM(AB6:AB8)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="1:28" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="40">
-        <f t="shared" ref="E10:M10" si="14">(E6+E7/2)/E9</f>
+      <c r="E10" s="36">
+        <f t="shared" ref="E10:G10" si="16">(E6+E7/2)/E9</f>
         <v>1</v>
       </c>
-      <c r="F10" s="40">
-        <f t="shared" si="14"/>
+      <c r="F10" s="36">
+        <f t="shared" si="16"/>
         <v>0.86842105263157898</v>
       </c>
-      <c r="G10" s="40">
-        <f t="shared" si="14"/>
+      <c r="G10" s="36">
+        <f t="shared" si="16"/>
         <v>0.57894736842105265</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="36">
         <f>(H6+H7/2)/H9</f>
         <v>0.56578947368421051</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="36">
         <f>(I6+I7/2)/I9</f>
         <v>0.59210526315789469</v>
       </c>
-      <c r="J10" s="40">
-        <f t="shared" ref="J10" si="15">(J6+J7/2)/J9</f>
+      <c r="J10" s="36">
+        <f t="shared" ref="J10" si="17">(J6+J7/2)/J9</f>
         <v>0.57894736842105265</v>
       </c>
-      <c r="K10" s="40">
-        <f t="shared" ref="K10:L10" si="16">(K6+K7/2)/K9</f>
+      <c r="K10" s="36">
+        <f t="shared" ref="K10:L10" si="18">(K6+K7/2)/K9</f>
         <v>0.51315789473684215</v>
       </c>
-      <c r="L10" s="40">
-        <f t="shared" si="16"/>
+      <c r="L10" s="36">
+        <f t="shared" si="18"/>
         <v>0.80263157894736847</v>
       </c>
-      <c r="M10" s="40">
-        <f t="shared" si="14"/>
+      <c r="M10" s="36">
+        <f t="shared" ref="M10" si="19">(M6+M7/2)/M9</f>
         <v>0.5</v>
       </c>
-      <c r="N10" s="40">
-        <f t="shared" ref="N10:P10" si="17">(N6+N7/2)/N9</f>
+      <c r="N10" s="36">
+        <f t="shared" ref="N10:Q10" si="20">(N6+N7/2)/N9</f>
         <v>0.53947368421052633</v>
       </c>
-      <c r="O10" s="40">
-        <f t="shared" si="17"/>
+      <c r="O10" s="36">
+        <f t="shared" si="20"/>
         <v>0.46052631578947367</v>
       </c>
-      <c r="P10" s="40">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q10" s="40">
-        <f t="shared" ref="Q10:T10" si="18">(Q6+Q7/2)/Q9</f>
-        <v>0.53947368421052633</v>
-      </c>
-      <c r="R10" s="40">
-        <f t="shared" si="18"/>
-        <v>0.46052631578947367</v>
-      </c>
-      <c r="S10" s="40">
-        <f t="shared" si="18"/>
+      <c r="P10" s="36">
+        <f t="shared" si="20"/>
         <v>0.48684210526315791</v>
       </c>
-      <c r="T10" s="40">
-        <f t="shared" si="18"/>
-        <v>0.43421052631578949</v>
-      </c>
-      <c r="U10" s="40">
-        <f t="shared" ref="U10:X10" si="19">(U6+U7/2)/U9</f>
-        <v>0.42105263157894735</v>
-      </c>
-      <c r="V10" s="40">
-        <f t="shared" si="19"/>
-        <v>0.53947368421052633</v>
-      </c>
-      <c r="W10" s="40">
-        <f t="shared" ref="W10:X10" si="20">(W6+W7/2)/W9</f>
-        <v>0.59210526315789469</v>
-      </c>
-      <c r="X10" s="40">
+      <c r="Q10" s="36">
         <f t="shared" si="20"/>
         <v>0.43421052631578949</v>
       </c>
-      <c r="Y10" s="40">
-        <f t="shared" ref="Y10" si="21">(Y6+Y7/2)/Y9</f>
+      <c r="R10" s="36">
+        <f t="shared" ref="R10:S10" si="21">(R6+R7/2)/R9</f>
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="S10" s="36">
+        <f t="shared" si="21"/>
+        <v>0.53947368421052633</v>
+      </c>
+      <c r="T10" s="36">
+        <f t="shared" ref="T10:U10" si="22">(T6+T7/2)/T9</f>
+        <v>0.59210526315789469</v>
+      </c>
+      <c r="U10" s="36">
+        <f t="shared" si="22"/>
+        <v>0.43421052631578949</v>
+      </c>
+      <c r="V10" s="36">
+        <f t="shared" ref="V10" si="23">(V6+V7/2)/V9</f>
         <v>0.5</v>
       </c>
-      <c r="Z10" s="40">
-        <f t="shared" ref="Z10:AB10" si="22">(Z6+Z7/2)/Z9</f>
+      <c r="W10" s="36">
+        <f t="shared" ref="W10:Y10" si="24">(W6+W7/2)/W9</f>
         <v>0.46052631578947367</v>
       </c>
-      <c r="AA10" s="40">
-        <f t="shared" si="22"/>
+      <c r="X10" s="36">
+        <f t="shared" si="24"/>
         <v>0.32894736842105265</v>
       </c>
-      <c r="AB10" s="40">
-        <f t="shared" si="22"/>
+      <c r="Y10" s="36">
+        <f t="shared" si="24"/>
         <v>0.60526315789473684</v>
+      </c>
+      <c r="Z10" s="36">
+        <f t="shared" ref="Z10:AB10" si="25">(Z6+Z7/2)/Z9</f>
+        <v>0.5</v>
+      </c>
+      <c r="AA10" s="36">
+        <f t="shared" si="25"/>
+        <v>0.53947368421052633</v>
+      </c>
+      <c r="AB10" s="36">
+        <f t="shared" si="25"/>
+        <v>0.46052631578947367</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -2144,20 +2127,18 @@
         <v>17</v>
       </c>
       <c r="L11" s="7"/>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="7"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="49"/>
+      <c r="Z11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="AA11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
+      <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
@@ -2187,17 +2168,17 @@
       <c r="K12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="R12" s="25"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="54"/>
+      <c r="Z12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="AA12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="U12" s="27"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="60"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>
@@ -2227,16 +2208,20 @@
       <c r="K13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="V13" s="51"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="AA13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
@@ -2264,10 +2249,10 @@
       <c r="K14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="Z14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="AA14" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2299,11 +2284,11 @@
       <c r="K15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="Z15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="7" t="s">
-        <v>150</v>
+      <c r="AA15" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
@@ -2325,23 +2310,23 @@
         <v>16</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="Z16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="AA16" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="6" t="s">
         <v>24</v>
@@ -2369,11 +2354,11 @@
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="Z17" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="6" t="s">
         <v>25</v>
@@ -2399,16 +2384,16 @@
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="M18" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -2426,10 +2411,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
       <c r="B20" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>17</v>
@@ -2442,118 +2427,100 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" s="24"/>
       <c r="B21" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="K21" s="47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="K21" s="51" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="51" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-    </row>
-    <row r="25" spans="1:13" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="6">
+      <c r="K22" s="47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="6">
         <v>1</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K23" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6">
         <v>2</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="6" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A11:S19 T11:XFD20 K11:L22 A20:R20 S20:S22">
+  <conditionalFormatting sqref="K11:L22 P20:P22 A11:P19 A20:O20 Q11:XFD20">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>LEFT(A11,1)="-"</formula>
     </cfRule>
@@ -2591,24 +2558,24 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2619,16 +2586,16 @@
         <v>46</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2639,16 +2606,16 @@
         <v>47</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2659,118 +2626,118 @@
         <v>48</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2778,13 +2745,13 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2792,7 +2759,7 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2800,7 +2767,7 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2808,10 +2775,10 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2819,13 +2786,13 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2833,13 +2800,13 @@
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2847,7 +2814,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2855,7 +2822,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2863,7 +2830,7 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2871,7 +2838,7 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2883,10 +2850,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADD34EC-FC63-4B23-9C13-E548752F8F18}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2908,19 +2875,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="38" t="s">
         <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>60</v>
@@ -2928,61 +2889,63 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>148</v>
-      </c>
-    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>143</v>
+      <c r="A7" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2996,7 +2959,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3995,53 +3958,53 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="39">
         <v>4</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="40">
         <v>3</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="40">
         <v>2</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="41">
         <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="37">
         <f>2*($F2)*(G$1)+ABS(G$7-$F8)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="41">
+      <c r="H2" s="37">
         <f t="shared" ref="H2:J2" si="0">2*($F2)*(H$1)+ABS(H$7-$F8)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="37">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J2" s="41">
+      <c r="J2" s="37">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="37">
         <f>ABS(B2-G2)</f>
         <v>4</v>
       </c>
-      <c r="M2" s="41">
+      <c r="M2" s="37">
         <f t="shared" ref="M2:O2" si="1">ABS(C2-H2)</f>
         <v>2</v>
       </c>
-      <c r="N2" s="41">
+      <c r="N2" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O2" s="41">
+      <c r="O2" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -4050,7 +4013,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="42">
         <v>3</v>
       </c>
       <c r="C3">
@@ -4059,48 +4022,48 @@
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="43">
         <v>5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="37">
         <f t="shared" ref="G3:J3" si="2">2*($F3)*(G$1)+ABS(G$7-$F9)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="41">
+      <c r="H3" s="37">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I3" s="41">
+      <c r="I3" s="37">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="37">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="37">
         <f t="shared" ref="L3:L5" si="3">ABS(B3-G3)</f>
         <v>2</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M3" s="37">
         <f t="shared" ref="M3:M5" si="4">ABS(C3-H3)</f>
         <v>5</v>
       </c>
-      <c r="N3" s="41">
+      <c r="N3" s="37">
         <f t="shared" ref="N3:N5" si="5">ABS(D3-I3)</f>
         <v>1</v>
       </c>
-      <c r="O3" s="41">
+      <c r="O3" s="37">
         <f t="shared" ref="O3:O5" si="6">ABS(E3-J3)</f>
         <v>3</v>
       </c>
-      <c r="Q3" s="41">
+      <c r="Q3" s="37">
         <f>SUM(L2:O5)</f>
         <v>44</v>
       </c>
@@ -4109,7 +4072,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="42">
         <v>2</v>
       </c>
       <c r="C4">
@@ -4118,44 +4081,44 @@
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="43">
         <v>8</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="37">
         <f t="shared" ref="G4:J4" si="7">2*($F4)*(G$1)+ABS(G$7-$F10)</f>
         <v>2</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="37">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4" s="37">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="37">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="37">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="37">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="37">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -4164,53 +4127,53 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="44">
         <v>1</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="45">
         <v>5</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="45">
         <v>8</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="46">
         <v>10</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="37">
         <f t="shared" ref="G5:J5" si="8">2*($F5)*(G$1)+ABS(G$7-$F11)</f>
         <v>3</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="37">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="37">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="37">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="37">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="37">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="37">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="37">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
@@ -4257,53 +4220,53 @@
       <c r="A8">
         <v>0</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="39">
         <v>4</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="40">
         <v>3</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="40">
         <v>2</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="41">
         <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="37">
         <f>4-ABS(G$7-$F8)+G$7*$F8</f>
         <v>4</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="37">
         <f t="shared" ref="H8:J11" si="9">4-ABS(H$7-$F8)+H$7*$F8</f>
         <v>3</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="37">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="37">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="37">
         <f>ABS(B8-G8)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="37">
         <f t="shared" ref="M8:M11" si="10">ABS(C8-H8)</f>
         <v>0</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="37">
         <f t="shared" ref="N8:N11" si="11">ABS(D8-I8)</f>
         <v>0</v>
       </c>
-      <c r="O8" s="41">
+      <c r="O8" s="37">
         <f t="shared" ref="O8:O11" si="12">ABS(E8-J8)</f>
         <v>0</v>
       </c>
@@ -4312,7 +4275,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="42">
         <v>3</v>
       </c>
       <c r="C9">
@@ -4321,48 +4284,48 @@
       <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="43">
         <v>5</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="37">
         <f t="shared" ref="G9:G11" si="13">4-ABS(G$7-$F9)+G$7*$F9</f>
         <v>3</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="37">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="37">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="37">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="37">
         <f t="shared" ref="L9:L11" si="14">ABS(B9-G9)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="37">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="37">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O9" s="41">
+      <c r="O9" s="37">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="41">
+      <c r="Q9" s="37">
         <f>SUM(L8:O11)</f>
         <v>10</v>
       </c>
@@ -4371,7 +4334,7 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="42">
         <v>2</v>
       </c>
       <c r="C10">
@@ -4380,44 +4343,44 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="43">
         <v>8</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="37">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="37">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10" s="37">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="37">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="37">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="37">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="N10" s="41">
+      <c r="N10" s="37">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O10" s="41">
+      <c r="O10" s="37">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
@@ -4426,53 +4389,53 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="44">
         <v>1</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="45">
         <v>5</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="45">
         <v>8</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="46">
         <v>10</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="37">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="37">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="37">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="37">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="37">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="37">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N11" s="41">
+      <c r="N11" s="37">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O11" s="41">
+      <c r="O11" s="37">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
@@ -4505,56 +4468,56 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="39">
         <v>1</v>
       </c>
-      <c r="O15" s="44">
+      <c r="O15" s="40">
         <v>2</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="40">
         <v>3</v>
       </c>
-      <c r="Q15" s="45">
+      <c r="Q15" s="41">
         <v>5</v>
       </c>
-      <c r="R15" s="43">
+      <c r="R15" s="39">
         <v>5</v>
       </c>
-      <c r="S15" s="44">
+      <c r="S15" s="40">
         <v>3</v>
       </c>
-      <c r="T15" s="44">
+      <c r="T15" s="40">
         <v>2</v>
       </c>
-      <c r="U15" s="45">
+      <c r="U15" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-      <c r="N16" s="46">
+      <c r="N16" s="42">
         <v>2</v>
       </c>
       <c r="O16">
@@ -4563,10 +4526,10 @@
       <c r="P16">
         <v>6</v>
       </c>
-      <c r="Q16" s="47">
+      <c r="Q16" s="43">
         <v>7</v>
       </c>
-      <c r="R16" s="46">
+      <c r="R16" s="42">
         <v>7</v>
       </c>
       <c r="S16">
@@ -4575,18 +4538,18 @@
       <c r="T16">
         <v>4</v>
       </c>
-      <c r="U16" s="47">
+      <c r="U16" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M17">
         <v>2</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="42">
         <v>3</v>
       </c>
       <c r="O17">
@@ -4595,10 +4558,10 @@
       <c r="P17">
         <v>8</v>
       </c>
-      <c r="Q17" s="47">
+      <c r="Q17" s="43">
         <v>9</v>
       </c>
-      <c r="R17" s="46">
+      <c r="R17" s="42">
         <v>9</v>
       </c>
       <c r="S17">
@@ -4607,71 +4570,71 @@
       <c r="T17">
         <v>6</v>
       </c>
-      <c r="U17" s="47">
+      <c r="U17" s="43">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="4:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M18">
         <v>3</v>
       </c>
-      <c r="N18" s="48">
+      <c r="N18" s="44">
         <v>5</v>
       </c>
-      <c r="O18" s="49">
+      <c r="O18" s="45">
         <v>7</v>
       </c>
-      <c r="P18" s="49">
+      <c r="P18" s="45">
         <v>9</v>
       </c>
-      <c r="Q18" s="50">
+      <c r="Q18" s="46">
         <v>10</v>
       </c>
-      <c r="R18" s="48">
+      <c r="R18" s="44">
         <v>10</v>
       </c>
-      <c r="S18" s="49">
+      <c r="S18" s="45">
         <v>9</v>
       </c>
-      <c r="T18" s="49">
+      <c r="T18" s="45">
         <v>7</v>
       </c>
-      <c r="U18" s="50">
+      <c r="U18" s="46">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M19">
         <v>4</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="39">
         <v>5</v>
       </c>
-      <c r="O19" s="44">
+      <c r="O19" s="40">
         <v>7</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="40">
         <v>9</v>
       </c>
-      <c r="Q19" s="45">
+      <c r="Q19" s="41">
         <v>10</v>
       </c>
-      <c r="R19" s="43">
+      <c r="R19" s="39">
         <v>10</v>
       </c>
-      <c r="S19" s="44">
+      <c r="S19" s="40">
         <v>9</v>
       </c>
-      <c r="T19" s="44">
+      <c r="T19" s="40">
         <v>7</v>
       </c>
-      <c r="U19" s="45">
+      <c r="U19" s="41">
         <v>5</v>
       </c>
     </row>
@@ -4679,7 +4642,7 @@
       <c r="M20">
         <v>5</v>
       </c>
-      <c r="N20" s="46">
+      <c r="N20" s="42">
         <v>3</v>
       </c>
       <c r="O20">
@@ -4688,10 +4651,10 @@
       <c r="P20">
         <v>8</v>
       </c>
-      <c r="Q20" s="47">
+      <c r="Q20" s="43">
         <v>9</v>
       </c>
-      <c r="R20" s="46">
+      <c r="R20" s="42">
         <v>9</v>
       </c>
       <c r="S20">
@@ -4700,7 +4663,7 @@
       <c r="T20">
         <v>6</v>
       </c>
-      <c r="U20" s="47">
+      <c r="U20" s="43">
         <v>3</v>
       </c>
     </row>
@@ -4708,7 +4671,7 @@
       <c r="M21">
         <v>6</v>
       </c>
-      <c r="N21" s="46">
+      <c r="N21" s="42">
         <v>2</v>
       </c>
       <c r="O21">
@@ -4717,10 +4680,10 @@
       <c r="P21">
         <v>6</v>
       </c>
-      <c r="Q21" s="47">
+      <c r="Q21" s="43">
         <v>7</v>
       </c>
-      <c r="R21" s="46">
+      <c r="R21" s="42">
         <v>7</v>
       </c>
       <c r="S21">
@@ -4729,7 +4692,7 @@
       <c r="T21">
         <v>4</v>
       </c>
-      <c r="U21" s="47">
+      <c r="U21" s="43">
         <v>2</v>
       </c>
     </row>
@@ -4737,28 +4700,28 @@
       <c r="M22">
         <v>7</v>
       </c>
-      <c r="N22" s="48">
+      <c r="N22" s="44">
         <v>1</v>
       </c>
-      <c r="O22" s="49">
+      <c r="O22" s="45">
         <v>2</v>
       </c>
-      <c r="P22" s="49">
+      <c r="P22" s="45">
         <v>3</v>
       </c>
-      <c r="Q22" s="50">
+      <c r="Q22" s="46">
         <v>5</v>
       </c>
-      <c r="R22" s="48">
+      <c r="R22" s="44">
         <v>5</v>
       </c>
-      <c r="S22" s="49">
+      <c r="S22" s="45">
         <v>3</v>
       </c>
-      <c r="T22" s="49">
+      <c r="T22" s="45">
         <v>2</v>
       </c>
-      <c r="U22" s="50">
+      <c r="U22" s="46">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first version, not working
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDesktop\Chess-Challange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C275484-134B-46CE-BD35-73C79B4AA8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FC7239-E8DC-4D35-A6B8-D4E964919813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparation" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="280">
   <si>
     <t>Random</t>
   </si>
@@ -906,6 +906,9 @@
   </si>
   <si>
     <t>V8.0</t>
+  </si>
+  <si>
+    <t>diagonal e implementata deja, mai trebuie doar la celelalte</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -4976,8 +4979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADD34EC-FC63-4B23-9C13-E548752F8F18}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5128,41 +5131,29 @@
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>152</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="37">
-        <v>0</v>
-      </c>
-      <c r="G18" s="38">
-        <v>9</v>
-      </c>
-      <c r="H18" s="38">
-        <v>17</v>
-      </c>
-      <c r="I18" s="39">
-        <v>30</v>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -5170,19 +5161,19 @@
         <v>153</v>
       </c>
       <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="40">
+        <v>0</v>
+      </c>
+      <c r="F19" s="37">
+        <v>0</v>
+      </c>
+      <c r="G19" s="38">
         <v>9</v>
       </c>
-      <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>35</v>
-      </c>
-      <c r="I19" s="41">
-        <v>39</v>
+      <c r="H19" s="38">
+        <v>17</v>
+      </c>
+      <c r="I19" s="39">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -5190,44 +5181,59 @@
         <v>188</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="40">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G20">
+        <v>24</v>
+      </c>
+      <c r="H20">
         <v>35</v>
       </c>
-      <c r="H20">
-        <v>42</v>
-      </c>
       <c r="I20" s="41">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>189</v>
       </c>
       <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21" s="42">
-        <v>30</v>
-      </c>
-      <c r="G21" s="43">
-        <v>39</v>
-      </c>
-      <c r="H21" s="43">
+        <v>2</v>
+      </c>
+      <c r="F21" s="40">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>42</v>
+      </c>
+      <c r="I21" s="41">
         <v>44</v>
       </c>
-      <c r="I21" s="44">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>272</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="42">
+        <v>30</v>
+      </c>
+      <c r="G22" s="43">
+        <v>39</v>
+      </c>
+      <c r="H22" s="43">
+        <v>44</v>
+      </c>
+      <c r="I22" s="44">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -7284,19 +7290,19 @@
         <v>0</v>
       </c>
       <c r="T3" s="37">
-        <f>0.5/(4-$S3)+0.5/(4-T$2)</f>
+        <f t="shared" ref="T3:W6" si="7">0.5/(4-$S3)+0.5/(4-T$2)</f>
         <v>0.25</v>
       </c>
       <c r="U3" s="37">
-        <f>0.5/(4-$S3)+0.5/(4-U$2)</f>
+        <f t="shared" si="7"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="V3" s="37">
-        <f>0.5/(4-$S3)+0.5/(4-V$2)</f>
+        <f t="shared" si="7"/>
         <v>0.375</v>
       </c>
       <c r="W3" s="37">
-        <f>0.5/(4-$S3)+0.5/(4-W$2)</f>
+        <f t="shared" si="7"/>
         <v>0.625</v>
       </c>
     </row>
@@ -7320,19 +7326,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="35">
-        <f t="shared" ref="G4:J4" si="7">2*($F4)*(G$1)+ABS(G$7-$F10)</f>
+        <f t="shared" ref="G4:J4" si="8">2*($F4)*(G$1)+ABS(G$7-$F10)</f>
         <v>2</v>
       </c>
       <c r="H4" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="I4" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="J4" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="K4">
@@ -7358,19 +7364,19 @@
         <v>1</v>
       </c>
       <c r="T4" s="37">
-        <f>0.5/(4-$S4)+0.5/(4-T$2)</f>
+        <f t="shared" si="7"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="U4" s="37">
-        <f>0.5/(4-$S4)+0.5/(4-U$2)</f>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="V4" s="37">
-        <f>0.5/(4-$S4)+0.5/(4-V$2)</f>
+        <f t="shared" si="7"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="W4" s="37">
-        <f>0.5/(4-$S4)+0.5/(4-W$2)</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -7394,19 +7400,19 @@
         <v>3</v>
       </c>
       <c r="G5" s="35">
-        <f t="shared" ref="G5:J5" si="8">2*($F5)*(G$1)+ABS(G$7-$F11)</f>
+        <f t="shared" ref="G5:J5" si="9">2*($F5)*(G$1)+ABS(G$7-$F11)</f>
         <v>3</v>
       </c>
       <c r="H5" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="I5" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="J5" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="K5">
@@ -7432,19 +7438,19 @@
         <v>2</v>
       </c>
       <c r="T5" s="37">
-        <f>0.5/(4-$S5)+0.5/(4-T$2)</f>
+        <f t="shared" si="7"/>
         <v>0.375</v>
       </c>
       <c r="U5" s="37">
-        <f>0.5/(4-$S5)+0.5/(4-U$2)</f>
+        <f t="shared" si="7"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="V5" s="37">
-        <f>0.5/(4-$S5)+0.5/(4-V$2)</f>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="W5" s="37">
-        <f>0.5/(4-$S5)+0.5/(4-W$2)</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
     </row>
@@ -7453,19 +7459,19 @@
         <v>3</v>
       </c>
       <c r="T6" s="37">
-        <f>0.5/(4-$S6)+0.5/(4-T$2)</f>
+        <f t="shared" si="7"/>
         <v>0.625</v>
       </c>
       <c r="U6" s="37">
-        <f>0.5/(4-$S6)+0.5/(4-U$2)</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="V6" s="37">
-        <f>0.5/(4-$S6)+0.5/(4-V$2)</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="W6" s="37">
-        <f>0.5/(4-$S6)+0.5/(4-W$2)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7531,15 +7537,15 @@
         <v>4</v>
       </c>
       <c r="H8" s="35">
-        <f t="shared" ref="H8:J11" si="9">4-ABS(H$7-$F8)+H$7*$F8</f>
+        <f t="shared" ref="H8:J11" si="10">4-ABS(H$7-$F8)+H$7*$F8</f>
         <v>3</v>
       </c>
       <c r="I8" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J8" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="K8">
@@ -7550,15 +7556,15 @@
         <v>0</v>
       </c>
       <c r="M8" s="35">
-        <f t="shared" ref="M8:M11" si="10">ABS(C8-H8)</f>
+        <f t="shared" ref="M8:M11" si="11">ABS(C8-H8)</f>
         <v>0</v>
       </c>
       <c r="N8" s="35">
-        <f t="shared" ref="N8:N11" si="11">ABS(D8-I8)</f>
+        <f t="shared" ref="N8:N11" si="12">ABS(D8-I8)</f>
         <v>0</v>
       </c>
       <c r="O8" s="35">
-        <f t="shared" ref="O8:O11" si="12">ABS(E8-J8)</f>
+        <f t="shared" ref="O8:O11" si="13">ABS(E8-J8)</f>
         <v>0</v>
       </c>
       <c r="T8">
@@ -7594,38 +7600,38 @@
         <v>1</v>
       </c>
       <c r="G9" s="35">
-        <f t="shared" ref="G9:G11" si="13">4-ABS(G$7-$F9)+G$7*$F9</f>
+        <f t="shared" ref="G9:G11" si="14">4-ABS(G$7-$F9)+G$7*$F9</f>
         <v>3</v>
       </c>
       <c r="H9" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="I9" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="J9" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" s="35">
-        <f t="shared" ref="L9:L11" si="14">ABS(B9-G9)</f>
+        <f t="shared" ref="L9:L11" si="15">ABS(B9-G9)</f>
         <v>0</v>
       </c>
       <c r="M9" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="N9" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="O9" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q9" s="35">
@@ -7640,15 +7646,15 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="U9" s="37">
-        <f t="shared" ref="U9:W12" si="15">1/(7-$S9-U$2)</f>
+        <f t="shared" ref="U9:W12" si="16">1/(7-$S9-U$2)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="V9" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.2</v>
       </c>
       <c r="W9" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.25</v>
       </c>
     </row>
@@ -7672,57 +7678,57 @@
         <v>2</v>
       </c>
       <c r="G10" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="H10" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="I10" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="J10" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
       <c r="L10" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M10" s="35">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="N10" s="35">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="O10" s="35">
+      <c r="N10" s="35">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
+      <c r="O10" s="35">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
       <c r="S10">
         <v>1</v>
       </c>
       <c r="T10" s="37">
-        <f t="shared" ref="T10:T12" si="16">1/(7-$S10-T$2)</f>
+        <f t="shared" ref="T10:T12" si="17">1/(7-$S10-T$2)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="U10" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.2</v>
       </c>
       <c r="V10" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.25</v>
       </c>
       <c r="W10" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -7746,57 +7752,57 @@
         <v>3</v>
       </c>
       <c r="G11" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="H11" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="I11" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="J11" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
       <c r="L11" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M11" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N11" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="O11" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="S11">
         <v>2</v>
       </c>
       <c r="T11" s="37">
+        <f t="shared" si="17"/>
+        <v>0.2</v>
+      </c>
+      <c r="U11" s="37">
         <f t="shared" si="16"/>
-        <v>0.2</v>
-      </c>
-      <c r="U11" s="37">
-        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="V11" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="W11" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
     </row>
@@ -7805,19 +7811,19 @@
         <v>3</v>
       </c>
       <c r="T12" s="37">
+        <f t="shared" si="17"/>
+        <v>0.25</v>
+      </c>
+      <c r="U12" s="37">
         <f t="shared" si="16"/>
-        <v>0.25</v>
-      </c>
-      <c r="U12" s="37">
-        <f t="shared" si="15"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="V12" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
       <c r="W12" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>